<commit_message>
Finish fibonacci heap assignment
</commit_message>
<xml_diff>
--- a/charles-university/data-structures-1/fibonacci-heap/docs/results-assignment-2.xlsx
+++ b/charles-university/data-structures-1/fibonacci-heap/docs/results-assignment-2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Heap Size</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>Naïve</t>
+  </si>
+  <si>
+    <t>Standard Heap</t>
   </si>
 </sst>
 </file>
@@ -131,8 +134,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Random Test</a:t>
+              <a:t>Random vs.</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Biased</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -168,8 +176,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -180,7 +188,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Standard</c:v>
+                  <c:v>Random Test</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -197,7 +205,7 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>results!$A$3:$A$22</c:f>
               <c:numCache>
@@ -265,76 +273,76 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>results!$B$3:$B$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>5.8041520000000002</c:v>
+                  <c:v>13.928330000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.9264020000000004</c:v>
+                  <c:v>14.292192999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.0076239999999999</c:v>
+                  <c:v>14.487869999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.0557480000000004</c:v>
+                  <c:v>14.620471</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.100949</c:v>
+                  <c:v>14.652310999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.1519320000000004</c:v>
+                  <c:v>14.802014</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.1621110000000003</c:v>
+                  <c:v>14.898175999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.1842790000000001</c:v>
+                  <c:v>14.892137999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.2143069999999998</c:v>
+                  <c:v>14.973976</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.228459</c:v>
+                  <c:v>14.997305000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6.24193</c:v>
+                  <c:v>15.007148000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.271401</c:v>
+                  <c:v>15.013442</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.2847080000000002</c:v>
+                  <c:v>15.06564</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.280386</c:v>
+                  <c:v>15.104606</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6.2851840000000001</c:v>
+                  <c:v>15.157202</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6.3229139999999999</c:v>
+                  <c:v>15.126300000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.3196950000000003</c:v>
+                  <c:v>15.187865</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.3365419999999997</c:v>
+                  <c:v>15.148281000000001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6.3374930000000003</c:v>
+                  <c:v>15.219144999999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6.3393810000000004</c:v>
+                  <c:v>15.200416000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -351,7 +359,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Naïve</c:v>
+                  <c:v>Biased Test</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -368,7 +376,7 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>results!$A$3:$A$22</c:f>
               <c:numCache>
@@ -436,76 +444,76 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>results!$C$3:$C$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>5.635853</c:v>
+                  <c:v>1255.9074069999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.7604730000000002</c:v>
+                  <c:v>1380.6632649999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.7855619999999996</c:v>
+                  <c:v>1438.1149829999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.8551460000000004</c:v>
+                  <c:v>1374.7686570000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.8834689999999998</c:v>
+                  <c:v>1382.6325300000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.9307210000000001</c:v>
+                  <c:v>1396.17479</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.9667339999999998</c:v>
+                  <c:v>1386.4575540000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.9782570000000002</c:v>
+                  <c:v>1429.5212899999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.9884370000000002</c:v>
+                  <c:v>1385.21</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.0036209999999999</c:v>
+                  <c:v>1417.9162409999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6.0165459999999999</c:v>
+                  <c:v>1461.545977</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.0295430000000003</c:v>
+                  <c:v>1423.617094</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.0514349999999997</c:v>
+                  <c:v>1381.9333329999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.083196</c:v>
+                  <c:v>1412.965091</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6.0810240000000002</c:v>
+                  <c:v>1402.686195</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6.1171720000000001</c:v>
+                  <c:v>1408.4385299999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.0927749999999996</c:v>
+                  <c:v>1375.200116</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.1183449999999997</c:v>
+                  <c:v>1413.458451</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6.1136530000000002</c:v>
+                  <c:v>1402.8339539999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6.1123310000000002</c:v>
+                  <c:v>1366.0270399999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -521,14 +529,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
         <c:axId val="641966232"/>
         <c:axId val="442491896"/>
-      </c:lineChart>
-      <c:catAx>
+      </c:scatterChart>
+      <c:valAx>
         <c:axId val="641966232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="2000000"/>
+          <c:min val="100000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -592,7 +601,7 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
-        <c:majorTickMark val="in"/>
+        <c:majorTickMark val="cross"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -630,17 +639,13 @@
         </c:txPr>
         <c:crossAx val="442491896"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
         <c:axId val="442491896"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
-          <c:max val="7"/>
-          <c:min val="5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -721,7 +726,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="#,##0.0" sourceLinked="0"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -755,7 +760,6 @@
         <c:crossAx val="641966232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="0.5"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -868,7 +872,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Biased Test</a:t>
+              <a:t>Special Test</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -905,8 +909,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -934,148 +938,190 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
-              <c:f>results!$A$26:$A$45</c:f>
+              <c:f>results!$A$26:$A$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
-                  <c:v>100000</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200000</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300000</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400000</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>500000</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>600000</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>700000</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>800000</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>900000</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000000</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1100000</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1200000</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1300000</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1400000</c:v>
+                  <c:v>108</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1500000</c:v>
+                  <c:v>123</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1600000</c:v>
+                  <c:v>139</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1700000</c:v>
+                  <c:v>156</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1800000</c:v>
+                  <c:v>174</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1900000</c:v>
+                  <c:v>193</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2000000</c:v>
+                  <c:v>213</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>234</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>279</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>303</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>328</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>354</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>381</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
-              <c:f>results!$B$26:$B$45</c:f>
+              <c:f>results!$B$26:$B$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
-                  <c:v>8.3695649999999997</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.9430049999999994</c:v>
+                  <c:v>1.987654</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.5645159999999994</c:v>
+                  <c:v>2.9512200000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.402469</c:v>
+                  <c:v>5.4217000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.3728160000000003</c:v>
+                  <c:v>5.9612999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.5423200000000001</c:v>
+                  <c:v>5.5432000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.5977340000000009</c:v>
+                  <c:v>5.9147999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.7140970000000006</c:v>
+                  <c:v>6.0006999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.8851770000000005</c:v>
+                  <c:v>6.1126E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.7947950000000006</c:v>
+                  <c:v>6.2571000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10.085046999999999</c:v>
+                  <c:v>6.3301999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9.4556959999999997</c:v>
+                  <c:v>6.3943E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9.9594919999999991</c:v>
+                  <c:v>6.4379000000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9.9643119999999996</c:v>
+                  <c:v>6.4645999999999995E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9.8618330000000007</c:v>
+                  <c:v>6.4670000000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9.7851289999999995</c:v>
+                  <c:v>6.4700999999999995E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9.8005929999999992</c:v>
+                  <c:v>6.4772999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9.9333690000000008</c:v>
+                  <c:v>6.4832000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>10.0625</c:v>
+                  <c:v>6.4859E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9.8676010000000005</c:v>
+                  <c:v>6.4880999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6.4894999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6.4896999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6.4894999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6.4893000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>6.4893000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6.4890000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6.4889000000000002E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2033-471A-80AB-59B0ACED1B5F}"/>
+              <c16:uniqueId val="{00000000-C410-4B53-99C2-BF4FD52827C5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1105,148 +1151,190 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
-              <c:f>results!$A$26:$A$45</c:f>
+              <c:f>results!$A$26:$A$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
-                  <c:v>100000</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200000</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300000</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400000</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>500000</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>600000</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>700000</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>800000</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>900000</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000000</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1100000</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1200000</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1300000</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1400000</c:v>
+                  <c:v>108</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1500000</c:v>
+                  <c:v>123</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1600000</c:v>
+                  <c:v>139</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1700000</c:v>
+                  <c:v>156</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1800000</c:v>
+                  <c:v>174</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1900000</c:v>
+                  <c:v>193</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2000000</c:v>
+                  <c:v>213</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>234</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>279</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>303</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>328</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>354</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>381</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
-              <c:f>results!$C$26:$C$45</c:f>
+              <c:f>results!$C$26:$C$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
-                  <c:v>8.4239130000000007</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.3264250000000004</c:v>
+                  <c:v>1.987654</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.4548389999999998</c:v>
+                  <c:v>2.9512200000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.4049379999999996</c:v>
+                  <c:v>3.8885540000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.3825240000000001</c:v>
+                  <c:v>4.8077500000000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.4263320000000004</c:v>
+                  <c:v>5.7184039999999996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.1558069999999994</c:v>
+                  <c:v>6.6274800000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.4255600000000008</c:v>
+                  <c:v>7.5387849999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.3841339999999995</c:v>
+                  <c:v>8.4537910000000007</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.3953950000000006</c:v>
+                  <c:v>9.3726029999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.4728969999999997</c:v>
+                  <c:v>10.294696</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9.3510550000000006</c:v>
+                  <c:v>11.219347000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9.6497220000000006</c:v>
+                  <c:v>12.145868999999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9.4770579999999995</c:v>
+                  <c:v>13.073696</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9.4589599999999994</c:v>
+                  <c:v>14.002402</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9.4341519999999992</c:v>
+                  <c:v>14.931683</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9.3637979999999992</c:v>
+                  <c:v>15.861331</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9.5034930000000006</c:v>
+                  <c:v>16.79121</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9.6310979999999997</c:v>
+                  <c:v>17.721229999999998</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9.5259610000000006</c:v>
+                  <c:v>18.651337000000002</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>19.581496000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>20.511686000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>21.441893</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>22.372112000000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>23.302336</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>24.232564</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>25.162794000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-2033-471A-80AB-59B0ACED1B5F}"/>
+              <c16:uniqueId val="{00000001-C410-4B53-99C2-BF4FD52827C5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1258,14 +1346,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
         <c:axId val="641966232"/>
         <c:axId val="442491896"/>
-      </c:lineChart>
-      <c:catAx>
+      </c:scatterChart>
+      <c:valAx>
         <c:axId val="641966232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="400"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1324,8 +1412,8 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
-        <c:majorTickMark val="in"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -1363,819 +1451,8 @@
         </c:txPr>
         <c:crossAx val="442491896"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="442491896"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="11"/>
-          <c:min val="8"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>ExtractMin Steps (Avg)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="#,##0.0" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="641966232"/>
-        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Special Test</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>results!$B$25</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Standard</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>results!$A$49:$A$75</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
-                <c:pt idx="0">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>58</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>69</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>81</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>94</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>108</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>123</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>139</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>156</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>174</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>193</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>213</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>234</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>279</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>303</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>328</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>354</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>381</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>results!$B$49:$B$75</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
-                <c:pt idx="0">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.98765400000000003</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.4634149999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.0239999999999998E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.9610000000000002E-3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.4349999999999997E-3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6.2449999999999997E-3</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4.9399999999999999E-3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5.5649999999999996E-3</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>6.1929999999999997E-3</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6.2319999999999997E-3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>6.5690000000000002E-3</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>6.8230000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>6.9490000000000003E-3</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>6.9239999999999996E-3</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>6.9410000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>7.0010000000000003E-3</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>7.0349999999999996E-3</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>7.0520000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>7.0590000000000002E-3</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>7.064E-3</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>7.0629999999999998E-3</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>7.0619999999999997E-3</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>7.0609999999999996E-3</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>7.0629999999999998E-3</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>7.0629999999999998E-3</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>7.0629999999999998E-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C410-4B53-99C2-BF4FD52827C5}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>results!$C$25</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Naïve</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>results!$A$49:$A$75</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
-                <c:pt idx="0">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>58</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>69</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>81</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>94</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>108</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>123</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>139</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>156</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>174</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>193</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>213</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>234</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>279</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>303</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>328</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>354</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>381</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>results!$C$49:$C$75</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
-                <c:pt idx="0">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.98765400000000003</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.4634149999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.927711</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.3845010000000002</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.8381370000000001</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.2916970000000001</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.7467980000000001</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4.2039960000000001</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4.6632360000000004</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5.124193</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5.5864700000000003</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>6.0497059999999996</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>6.5136060000000002</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>6.9779530000000003</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>7.4425889999999999</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>7.9074119999999999</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>8.3723500000000008</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>8.8373600000000003</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>9.3024129999999996</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>9.7674920000000007</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>10.232587000000001</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>10.697691000000001</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>11.162800000000001</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>11.627912</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>12.093026</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>12.558141000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-C410-4B53-99C2-BF4FD52827C5}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="641966232"/>
-        <c:axId val="442491896"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="641966232"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Heap Size (n)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
-        <c:majorTickMark val="in"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="442491896"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
       <c:valAx>
         <c:axId val="442491896"/>
         <c:scaling>
@@ -2449,46 +1726,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -3521,536 +2758,20 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>971550</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4077,53 +2798,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F844F28-CFB0-4BB0-A3FF-73D339BE6621}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>47</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>981075</xdr:colOff>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4145,7 +2828,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4159,28 +2842,16 @@
   <autoFilter ref="A2:C22" xr:uid="{D3B23E46-DAE5-44F8-A892-78F239B698BD}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{50771C41-7047-4930-BC94-61CDD3E8D0FF}" name="Heap Size"/>
-    <tableColumn id="2" xr3:uid="{14BCE53E-29D3-43FC-AF43-D619A67C748C}" name="Standard"/>
-    <tableColumn id="3" xr3:uid="{FD857AD9-B437-468D-82FC-5CA470A5D8BB}" name="Naïve"/>
+    <tableColumn id="2" xr3:uid="{14BCE53E-29D3-43FC-AF43-D619A67C748C}" name="Random Test"/>
+    <tableColumn id="3" xr3:uid="{FD857AD9-B437-468D-82FC-5CA470A5D8BB}" name="Biased Test"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A563DDC5-AE43-40B4-80FC-24A0836DCF09}" name="Table2" displayName="Table2" ref="A25:C45" totalsRowShown="0">
-  <autoFilter ref="A25:C45" xr:uid="{E029DBD8-E93F-4AD4-AA9D-71BF8F50BCC7}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{7AD5AC56-58AC-40C1-9B8D-3E3E894DA4C8}" name="Heap Size"/>
-    <tableColumn id="2" xr3:uid="{820063D7-6D33-4584-8DFB-81501130541C}" name="Standard"/>
-    <tableColumn id="3" xr3:uid="{7CEB1DF4-7939-4548-8B61-7D664BDE24BA}" name="Naïve"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A404CFA6-0E25-4ABF-BB29-9B0D5EFF9634}" name="Table3" displayName="Table3" ref="A48:C75" totalsRowShown="0">
-  <autoFilter ref="A48:C75" xr:uid="{727AA12B-3B73-4DA7-B98C-E2A9915F775D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A404CFA6-0E25-4ABF-BB29-9B0D5EFF9634}" name="Table3" displayName="Table3" ref="A25:C52" totalsRowShown="0">
+  <autoFilter ref="A25:C52" xr:uid="{727AA12B-3B73-4DA7-B98C-E2A9915F775D}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{DCC397BB-FC2E-4147-9199-4F59078EEEE5}" name="Heap Size"/>
     <tableColumn id="2" xr3:uid="{3E52EDD1-E9A0-46E0-8291-C0F800E0A749}" name="Standard"/>
@@ -4487,10 +3158,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14837F66-51A8-4B5C-A2C1-2C2554CC75DD}">
-  <dimension ref="A1:F75"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4499,267 +3170,255 @@
     <col min="2" max="2" width="25.42578125" customWidth="1"/>
     <col min="3" max="3" width="22.7109375" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="7" max="7" width="25.42578125" customWidth="1"/>
-    <col min="8" max="8" width="22.7109375" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
     <col min="11" max="11" width="11.7109375" customWidth="1"/>
     <col min="12" max="12" width="25.42578125" customWidth="1"/>
     <col min="13" max="13" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>100000</v>
       </c>
       <c r="B3">
-        <v>5.8041520000000002</v>
+        <v>13.928330000000001</v>
       </c>
       <c r="C3">
-        <v>5.635853</v>
-      </c>
-      <c r="E3">
-        <f>SUM(Table1[Standard])</f>
-        <v>123.85559699999999</v>
-      </c>
-      <c r="F3">
-        <f>SUM(Table1[Naïve])</f>
-        <v>119.60429300000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1255.9074069999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>200000</v>
       </c>
       <c r="B4">
-        <v>5.9264020000000004</v>
+        <v>14.292192999999999</v>
       </c>
       <c r="C4">
-        <v>5.7604730000000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1380.6632649999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>300000</v>
       </c>
       <c r="B5">
-        <v>6.0076239999999999</v>
+        <v>14.487869999999999</v>
       </c>
       <c r="C5">
-        <v>5.7855619999999996</v>
-      </c>
-      <c r="E5">
-        <f>E3/F3</f>
-        <v>1.0355447442007786</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1438.1149829999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>400000</v>
       </c>
       <c r="B6">
-        <v>6.0557480000000004</v>
+        <v>14.620471</v>
       </c>
       <c r="C6">
-        <v>5.8551460000000004</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1374.7686570000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>500000</v>
       </c>
       <c r="B7">
-        <v>6.100949</v>
+        <v>14.652310999999999</v>
       </c>
       <c r="C7">
-        <v>5.8834689999999998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1382.6325300000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>600000</v>
       </c>
       <c r="B8">
-        <v>6.1519320000000004</v>
+        <v>14.802014</v>
       </c>
       <c r="C8">
-        <v>5.9307210000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1396.17479</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>700000</v>
       </c>
       <c r="B9">
-        <v>6.1621110000000003</v>
+        <v>14.898175999999999</v>
       </c>
       <c r="C9">
-        <v>5.9667339999999998</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1386.4575540000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>800000</v>
       </c>
       <c r="B10">
-        <v>6.1842790000000001</v>
+        <v>14.892137999999999</v>
       </c>
       <c r="C10">
-        <v>5.9782570000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1429.5212899999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>900000</v>
       </c>
       <c r="B11">
-        <v>6.2143069999999998</v>
+        <v>14.973976</v>
       </c>
       <c r="C11">
-        <v>5.9884370000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1385.21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1000000</v>
       </c>
       <c r="B12">
-        <v>6.228459</v>
+        <v>14.997305000000001</v>
       </c>
       <c r="C12">
-        <v>6.0036209999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1417.9162409999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1100000</v>
       </c>
       <c r="B13">
-        <v>6.24193</v>
+        <v>15.007148000000001</v>
       </c>
       <c r="C13">
-        <v>6.0165459999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1461.545977</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1200000</v>
       </c>
       <c r="B14">
-        <v>6.271401</v>
+        <v>15.013442</v>
       </c>
       <c r="C14">
-        <v>6.0295430000000003</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1423.617094</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1300000</v>
       </c>
       <c r="B15">
-        <v>6.2847080000000002</v>
+        <v>15.06564</v>
       </c>
       <c r="C15">
-        <v>6.0514349999999997</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1381.9333329999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1400000</v>
       </c>
       <c r="B16">
-        <v>6.280386</v>
+        <v>15.104606</v>
       </c>
       <c r="C16">
-        <v>6.083196</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1412.965091</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1500000</v>
       </c>
       <c r="B17">
-        <v>6.2851840000000001</v>
+        <v>15.157202</v>
       </c>
       <c r="C17">
-        <v>6.0810240000000002</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1402.686195</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1600000</v>
       </c>
       <c r="B18">
-        <v>6.3229139999999999</v>
+        <v>15.126300000000001</v>
       </c>
       <c r="C18">
-        <v>6.1171720000000001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1408.4385299999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1700000</v>
       </c>
       <c r="B19">
-        <v>6.3196950000000003</v>
+        <v>15.187865</v>
       </c>
       <c r="C19">
-        <v>6.0927749999999996</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1375.200116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1800000</v>
       </c>
       <c r="B20">
-        <v>6.3365419999999997</v>
+        <v>15.148281000000001</v>
       </c>
       <c r="C20">
-        <v>6.1183449999999997</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1413.458451</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1900000</v>
       </c>
       <c r="B21">
-        <v>6.3374930000000003</v>
+        <v>15.219144999999999</v>
       </c>
       <c r="C21">
-        <v>6.1136530000000002</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1402.8339539999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2000000</v>
       </c>
       <c r="B22">
-        <v>6.3393810000000004</v>
+        <v>15.200416000000001</v>
       </c>
       <c r="C22">
-        <v>6.1123310000000002</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1366.0270399999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -4770,570 +3429,309 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>100000</v>
+        <v>4</v>
       </c>
       <c r="B26">
-        <v>8.3695649999999997</v>
+        <v>1</v>
       </c>
       <c r="C26">
-        <v>8.4239130000000007</v>
-      </c>
-      <c r="E26">
-        <f>SUM(Table2[Standard])</f>
-        <v>192.96206600000002</v>
-      </c>
-      <c r="F26">
-        <f>SUM(Table2[Naïve])</f>
-        <v>186.64806099999998</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>200000</v>
+        <v>6</v>
       </c>
       <c r="B27">
-        <v>8.9430049999999994</v>
+        <v>1.987654</v>
       </c>
       <c r="C27">
-        <v>8.3264250000000004</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.987654</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>300000</v>
+        <v>9</v>
       </c>
       <c r="B28">
-        <v>9.5645159999999994</v>
+        <v>2.9512200000000002</v>
       </c>
       <c r="C28">
-        <v>9.4548389999999998</v>
-      </c>
-      <c r="E28">
-        <f>E26/F26</f>
-        <v>1.0338283985709342</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2.9512200000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>400000</v>
+        <v>13</v>
       </c>
       <c r="B29">
-        <v>9.402469</v>
+        <v>5.4217000000000001E-2</v>
       </c>
       <c r="C29">
-        <v>9.4049379999999996</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3.8885540000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>500000</v>
+        <v>18</v>
       </c>
       <c r="B30">
-        <v>9.3728160000000003</v>
+        <v>5.9612999999999999E-2</v>
       </c>
       <c r="C30">
-        <v>9.3825240000000001</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4.8077500000000004</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>600000</v>
+        <v>24</v>
       </c>
       <c r="B31">
-        <v>9.5423200000000001</v>
+        <v>5.5432000000000002E-2</v>
       </c>
       <c r="C31">
-        <v>9.4263320000000004</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5.7184039999999996</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>700000</v>
+        <v>31</v>
       </c>
       <c r="B32">
-        <v>9.5977340000000009</v>
+        <v>5.9147999999999999E-2</v>
       </c>
       <c r="C32">
-        <v>9.1558069999999994</v>
+        <v>6.6274800000000003</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>800000</v>
+        <v>39</v>
       </c>
       <c r="B33">
-        <v>9.7140970000000006</v>
+        <v>6.0006999999999998E-2</v>
       </c>
       <c r="C33">
-        <v>9.4255600000000008</v>
+        <v>7.5387849999999998</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>900000</v>
+        <v>48</v>
       </c>
       <c r="B34">
-        <v>9.8851770000000005</v>
+        <v>6.1126E-2</v>
       </c>
       <c r="C34">
-        <v>9.3841339999999995</v>
+        <v>8.4537910000000007</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>1000000</v>
+        <v>58</v>
       </c>
       <c r="B35">
-        <v>9.7947950000000006</v>
+        <v>6.2571000000000002E-2</v>
       </c>
       <c r="C35">
-        <v>9.3953950000000006</v>
+        <v>9.3726029999999998</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>1100000</v>
+        <v>69</v>
       </c>
       <c r="B36">
-        <v>10.085046999999999</v>
+        <v>6.3301999999999997E-2</v>
       </c>
       <c r="C36">
-        <v>9.4728969999999997</v>
+        <v>10.294696</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>1200000</v>
+        <v>81</v>
       </c>
       <c r="B37">
-        <v>9.4556959999999997</v>
+        <v>6.3943E-2</v>
       </c>
       <c r="C37">
-        <v>9.3510550000000006</v>
+        <v>11.219347000000001</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>1300000</v>
+        <v>94</v>
       </c>
       <c r="B38">
-        <v>9.9594919999999991</v>
+        <v>6.4379000000000006E-2</v>
       </c>
       <c r="C38">
-        <v>9.6497220000000006</v>
+        <v>12.145868999999999</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>1400000</v>
+        <v>108</v>
       </c>
       <c r="B39">
-        <v>9.9643119999999996</v>
+        <v>6.4645999999999995E-2</v>
       </c>
       <c r="C39">
-        <v>9.4770579999999995</v>
+        <v>13.073696</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>1500000</v>
+        <v>123</v>
       </c>
       <c r="B40">
-        <v>9.8618330000000007</v>
+        <v>6.4670000000000005E-2</v>
       </c>
       <c r="C40">
-        <v>9.4589599999999994</v>
+        <v>14.002402</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>1600000</v>
+        <v>139</v>
       </c>
       <c r="B41">
-        <v>9.7851289999999995</v>
+        <v>6.4700999999999995E-2</v>
       </c>
       <c r="C41">
-        <v>9.4341519999999992</v>
+        <v>14.931683</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>1700000</v>
+        <v>156</v>
       </c>
       <c r="B42">
-        <v>9.8005929999999992</v>
+        <v>6.4772999999999997E-2</v>
       </c>
       <c r="C42">
-        <v>9.3637979999999992</v>
+        <v>15.861331</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>1800000</v>
+        <v>174</v>
       </c>
       <c r="B43">
-        <v>9.9333690000000008</v>
+        <v>6.4832000000000001E-2</v>
       </c>
       <c r="C43">
-        <v>9.5034930000000006</v>
+        <v>16.79121</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>1900000</v>
+        <v>193</v>
       </c>
       <c r="B44">
-        <v>10.0625</v>
+        <v>6.4859E-2</v>
       </c>
       <c r="C44">
-        <v>9.6310979999999997</v>
+        <v>17.721229999999998</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>2000000</v>
+        <v>213</v>
       </c>
       <c r="B45">
-        <v>9.8676010000000005</v>
+        <v>6.4880999999999994E-2</v>
       </c>
       <c r="C45">
-        <v>9.5259610000000006</v>
+        <v>18.651337000000002</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>234</v>
+      </c>
+      <c r="B46">
+        <v>6.4894999999999994E-2</v>
+      </c>
+      <c r="C46">
+        <v>19.581496000000001</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>3</v>
+      <c r="A47">
+        <v>256</v>
+      </c>
+      <c r="B47">
+        <v>6.4896999999999996E-2</v>
+      </c>
+      <c r="C47">
+        <v>20.511686000000001</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>0</v>
-      </c>
-      <c r="B48" t="s">
-        <v>4</v>
-      </c>
-      <c r="C48" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>279</v>
+      </c>
+      <c r="B48">
+        <v>6.4894999999999994E-2</v>
+      </c>
+      <c r="C48">
+        <v>21.441893</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>4</v>
+        <v>303</v>
       </c>
       <c r="B49">
-        <v>0.5</v>
+        <v>6.4893000000000006E-2</v>
       </c>
       <c r="C49">
-        <v>0.5</v>
-      </c>
-      <c r="E49">
-        <f>SUM(Table3[Standard])</f>
-        <v>3.1084559999999994</v>
-      </c>
-      <c r="F49">
-        <f>SUM(Table3[Naïve])</f>
-        <v>176.26084600000002</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+        <v>22.372112000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>6</v>
+        <v>328</v>
       </c>
       <c r="B50">
-        <v>0.98765400000000003</v>
+        <v>6.4893000000000006E-2</v>
       </c>
       <c r="C50">
-        <v>0.98765400000000003</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+        <v>23.302336</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>9</v>
+        <v>354</v>
       </c>
       <c r="B51">
-        <v>1.4634149999999999</v>
+        <v>6.4890000000000003E-2</v>
       </c>
       <c r="C51">
-        <v>1.4634149999999999</v>
-      </c>
-      <c r="E51">
-        <f>E49/F49</f>
-        <v>1.7635544538348574E-2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+        <v>24.232564</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>13</v>
+        <v>381</v>
       </c>
       <c r="B52">
-        <v>6.0239999999999998E-3</v>
+        <v>6.4889000000000002E-2</v>
       </c>
       <c r="C52">
-        <v>1.927711</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>18</v>
-      </c>
-      <c r="B53">
-        <v>5.9610000000000002E-3</v>
-      </c>
-      <c r="C53">
-        <v>2.3845010000000002</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>24</v>
-      </c>
-      <c r="B54">
-        <v>4.4349999999999997E-3</v>
-      </c>
-      <c r="C54">
-        <v>2.8381370000000001</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>31</v>
-      </c>
-      <c r="B55">
-        <v>6.2449999999999997E-3</v>
-      </c>
-      <c r="C55">
-        <v>3.2916970000000001</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>39</v>
-      </c>
-      <c r="B56">
-        <v>4.9399999999999999E-3</v>
-      </c>
-      <c r="C56">
-        <v>3.7467980000000001</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>48</v>
-      </c>
-      <c r="B57">
-        <v>5.5649999999999996E-3</v>
-      </c>
-      <c r="C57">
-        <v>4.2039960000000001</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>58</v>
-      </c>
-      <c r="B58">
-        <v>6.1929999999999997E-3</v>
-      </c>
-      <c r="C58">
-        <v>4.6632360000000004</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>69</v>
-      </c>
-      <c r="B59">
-        <v>6.2319999999999997E-3</v>
-      </c>
-      <c r="C59">
-        <v>5.124193</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>81</v>
-      </c>
-      <c r="B60">
-        <v>6.5690000000000002E-3</v>
-      </c>
-      <c r="C60">
-        <v>5.5864700000000003</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>94</v>
-      </c>
-      <c r="B61">
-        <v>6.8230000000000001E-3</v>
-      </c>
-      <c r="C61">
-        <v>6.0497059999999996</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>108</v>
-      </c>
-      <c r="B62">
-        <v>6.9490000000000003E-3</v>
-      </c>
-      <c r="C62">
-        <v>6.5136060000000002</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>123</v>
-      </c>
-      <c r="B63">
-        <v>6.9239999999999996E-3</v>
-      </c>
-      <c r="C63">
-        <v>6.9779530000000003</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>139</v>
-      </c>
-      <c r="B64">
-        <v>6.9410000000000001E-3</v>
-      </c>
-      <c r="C64">
-        <v>7.4425889999999999</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>156</v>
-      </c>
-      <c r="B65">
-        <v>7.0010000000000003E-3</v>
-      </c>
-      <c r="C65">
-        <v>7.9074119999999999</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>174</v>
-      </c>
-      <c r="B66">
-        <v>7.0349999999999996E-3</v>
-      </c>
-      <c r="C66">
-        <v>8.3723500000000008</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <v>193</v>
-      </c>
-      <c r="B67">
-        <v>7.0520000000000001E-3</v>
-      </c>
-      <c r="C67">
-        <v>8.8373600000000003</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <v>213</v>
-      </c>
-      <c r="B68">
-        <v>7.0590000000000002E-3</v>
-      </c>
-      <c r="C68">
-        <v>9.3024129999999996</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69">
-        <v>234</v>
-      </c>
-      <c r="B69">
-        <v>7.064E-3</v>
-      </c>
-      <c r="C69">
-        <v>9.7674920000000007</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70">
-        <v>256</v>
-      </c>
-      <c r="B70">
-        <v>7.0629999999999998E-3</v>
-      </c>
-      <c r="C70">
-        <v>10.232587000000001</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71">
-        <v>279</v>
-      </c>
-      <c r="B71">
-        <v>7.0619999999999997E-3</v>
-      </c>
-      <c r="C71">
-        <v>10.697691000000001</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72">
-        <v>303</v>
-      </c>
-      <c r="B72">
-        <v>7.0609999999999996E-3</v>
-      </c>
-      <c r="C72">
-        <v>11.162800000000001</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73">
-        <v>328</v>
-      </c>
-      <c r="B73">
-        <v>7.0629999999999998E-3</v>
-      </c>
-      <c r="C73">
-        <v>11.627912</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74">
-        <v>354</v>
-      </c>
-      <c r="B74">
-        <v>7.0629999999999998E-3</v>
-      </c>
-      <c r="C74">
-        <v>12.093026</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>381</v>
-      </c>
-      <c r="B75">
-        <v>7.0629999999999998E-3</v>
-      </c>
-      <c r="C75">
-        <v>12.558141000000001</v>
+        <v>25.162794000000002</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-  <tableParts count="3">
+  <tableParts count="2">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
-    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>